<commit_message>
Actualizado power y operational_mode
</commit_message>
<xml_diff>
--- a/AutomationFramework/excel_logs/hardware_test_hw_component_test_hw_component_partnumber_logs.xlsx
+++ b/AutomationFramework/excel_logs/hardware_test_hw_component_test_hw_component_partnumber_logs.xlsx
@@ -497,10 +497,44 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>&lt;get&gt;
+  &lt;filter&gt;
+    &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+      &lt;component&gt;
+        &lt;name&gt;Waveserver-Ai&lt;/name&gt;
+        &lt;state&gt;
+          &lt;part-no&gt;&lt;/part-no&gt;
+        &lt;/state&gt;
+      &lt;/component&gt;
+    &lt;/components&gt;
+  &lt;/filter&gt;
+&lt;/get&gt;</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;rpc-reply message-id="urn:uuid:e6891d16-81b1-44eb-8d42-93065de7beed"
+ xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
+ ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
+ xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+ &lt;data&gt;
+  &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+   &lt;component&gt;
+    &lt;name&gt;Waveserver-Ai&lt;/name&gt;
+    &lt;state&gt;
+     &lt;part-no&gt;186-1010-900&lt;/part-no&gt;
+    &lt;/state&gt;
+   &lt;/component&gt;
+  &lt;/components&gt;
+ &lt;/data&gt;
+&lt;/rpc-reply&gt;</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>